<commit_message>
add yellow line which should represent one-part pipe
</commit_message>
<xml_diff>
--- a/dizajn valjda.xlsx
+++ b/dizajn valjda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlaki\Desktop\petnica-flappybird-asm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F60BB3-EB5B-42A3-8826-3B463A91EFB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAACBE22-8EE5-46B1-8547-79BF8F236D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{F8FF2C08-8F28-404E-9004-67F14204EE7A}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:AL24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -631,8 +631,8 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>

</xml_diff>